<commit_message>
fix import and export
</commit_message>
<xml_diff>
--- a/public/uploads/excel/guard.xlsx
+++ b/public/uploads/excel/guard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Micole\hostel management system\excel import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A2CFB8A-286F-497D-AB77-366FE61A8063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5746921-2B75-4BAD-9141-A1B2556DFCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{04BABEA2-8504-46BB-AAB6-D8B3B1ED2E0B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{15EDEDBA-FF3A-4374-9F45-4E4BC5AC95E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,46 +36,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Nama</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>nama</t>
   </si>
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>No. Tel Bimbit</t>
-  </si>
-  <si>
-    <t>guard 2</t>
-  </si>
-  <si>
-    <t>guard 3</t>
-  </si>
-  <si>
-    <t>guard 4</t>
-  </si>
-  <si>
-    <t>guard 5</t>
-  </si>
-  <si>
-    <t>guard2@gmail.com</t>
-  </si>
-  <si>
-    <t>guard3@gmail.com</t>
-  </si>
-  <si>
-    <t>guard4@gmail.com</t>
-  </si>
-  <si>
-    <t>guard5@gmail.com</t>
+    <t>no_tel_bimbit</t>
+  </si>
+  <si>
+    <t>testguard4</t>
+  </si>
+  <si>
+    <t>testguard5</t>
+  </si>
+  <si>
+    <t>testguard6</t>
+  </si>
+  <si>
+    <t>0102023321</t>
+  </si>
+  <si>
+    <t>0102023322</t>
+  </si>
+  <si>
+    <t>0102023323</t>
+  </si>
+  <si>
+    <t>testguard5@gmail.com</t>
+  </si>
+  <si>
+    <t>testguard4@gmail.com</t>
+  </si>
+  <si>
+    <t>testguard6@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +90,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,9 +122,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -430,16 +440,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC606AD9-D53A-4E15-81DA-421361B32451}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36D8B0E-AA7C-4889-A687-A12DD2B8A51E}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -447,63 +459,56 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>101122325</v>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>123232623</v>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>156655857</v>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>136633657</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{140E44B8-717C-4FCF-AE0A-1DB194A02719}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{76A06D1D-F334-44C2-A5B9-7D973EF4294C}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{4FDA708E-00E6-4C6E-B6D0-1D1AE7CD93F1}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{6E903A54-E48D-46E9-A975-DD93E09386B7}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{9ECFA64B-7484-47C0-A44E-152AD0AA2E58}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{4721B202-3768-446D-9BC3-AD51F2AA3D21}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{B2B5CC69-296F-4AB9-851B-CF65364A09D9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>